<commit_message>
My Day 2 first commit for the Ebay app project
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QEACOE\EBayDemo\EBay\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12135" windowHeight="4455"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -33,6 +29,9 @@
   </si>
   <si>
     <t>TCID</t>
+  </si>
+  <si>
+    <t>SearchPassword</t>
   </si>
 </sst>
 </file>
@@ -350,15 +349,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D1"/>
+  <dimension ref="B1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -368,6 +370,9 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Day 2 second commit for Ebay app
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12135" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14505" windowHeight="6015"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestDataSheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Username</t>
   </si>
@@ -31,17 +31,37 @@
     <t>TCID</t>
   </si>
   <si>
-    <t>SearchPassword</t>
+    <t>SearchProduct</t>
+  </si>
+  <si>
+    <t>TC01</t>
+  </si>
+  <si>
+    <t>tariq19ansari@gmail.com</t>
+  </si>
+  <si>
+    <t>Qwerty123</t>
+  </si>
+  <si>
+    <t>Julius Caesar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -64,13 +84,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -349,32 +372,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>